<commit_message>
AIP-629 AIP-640 Test Data Files
</commit_message>
<xml_diff>
--- a/Carrick_AutomatedTest/Carrick_Automation/TestData/CablingDataSet/CablingDataSet_18Channel/3U.xlsx
+++ b/Carrick_AutomatedTest/Carrick_Automation/TestData/CablingDataSet/CablingDataSet_18Channel/3U.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A7EF04-877C-4117-B9E9-6D65C65C73C2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{561C713A-6FDC-42DB-B272-ECA41B8AE72D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DeviceInfo" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1914" uniqueCount="1788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1918" uniqueCount="1792">
   <si>
     <t>Channel</t>
   </si>
@@ -5389,6 +5389,18 @@
   </si>
   <si>
     <t>DSP_2_Feeder_Map_2</t>
+  </si>
+  <si>
+    <t>DeviceType</t>
+  </si>
+  <si>
+    <t>DeviceName</t>
+  </si>
+  <si>
+    <t>IDM+18</t>
+  </si>
+  <si>
+    <t>IND_DAU_51</t>
   </si>
 </sst>
 </file>
@@ -5424,9 +5436,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -5720,10 +5730,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F923C6E4-9180-482F-96F8-7DC1FEB48257}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5732,20 +5742,32 @@
     <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>76</v>
       </c>
       <c r="B1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>1788</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1789</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>78</v>
       </c>
       <c r="B2" t="s">
         <v>79</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1790</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1791</v>
       </c>
     </row>
   </sheetData>
@@ -6560,7 +6582,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
@@ -6596,7 +6618,7 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2">
         <v>1</v>
       </c>
     </row>
@@ -6610,7 +6632,7 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3">
         <v>2</v>
       </c>
     </row>
@@ -6624,7 +6646,7 @@
       <c r="C4">
         <v>2</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4">
         <v>3</v>
       </c>
     </row>
@@ -6638,7 +6660,7 @@
       <c r="C5">
         <v>3</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5">
         <v>13</v>
       </c>
     </row>
@@ -6652,7 +6674,7 @@
       <c r="C6">
         <v>4</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6">
         <v>14</v>
       </c>
     </row>
@@ -6666,7 +6688,7 @@
       <c r="C7">
         <v>5</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7">
         <v>15</v>
       </c>
     </row>
@@ -6680,7 +6702,7 @@
       <c r="C8">
         <v>6</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8">
         <v>16</v>
       </c>
     </row>
@@ -6694,7 +6716,7 @@
       <c r="C9">
         <v>7</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9">
         <v>17</v>
       </c>
     </row>
@@ -6708,7 +6730,7 @@
       <c r="C10">
         <v>8</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10">
         <v>18</v>
       </c>
     </row>
@@ -15544,58 +15566,58 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" t="s">
         <v>1781</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>1739</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>1782</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>1783</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>1784</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" t="s">
         <v>1785</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" t="s">
         <v>1786</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" t="s">
         <v>1787</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7">
         <v>-1</v>
       </c>
     </row>
@@ -15619,135 +15641,135 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>1740</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1739</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>1741</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>1742</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>1743</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>1744</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>1745</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>1746</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>1747</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>1748</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>1749</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>1750</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>1751</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>1752</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>1753</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14">
         <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>1754</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>1755</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>1756</v>
       </c>
       <c r="B17">
@@ -15755,7 +15777,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>1757</v>
       </c>
       <c r="B18">
@@ -15763,7 +15785,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>1758</v>
       </c>
       <c r="B19">
@@ -15771,7 +15793,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>1759</v>
       </c>
       <c r="B20">
@@ -15779,7 +15801,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>1760</v>
       </c>
       <c r="B21">
@@ -15787,7 +15809,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>1761</v>
       </c>
       <c r="B22">
@@ -15795,7 +15817,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>1762</v>
       </c>
       <c r="B23">
@@ -15803,7 +15825,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>1763</v>
       </c>
       <c r="B24">
@@ -15811,7 +15833,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>1764</v>
       </c>
       <c r="B25">
@@ -15819,7 +15841,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>1765</v>
       </c>
       <c r="B26">
@@ -15827,7 +15849,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
         <v>1766</v>
       </c>
       <c r="B27">
@@ -15835,7 +15857,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
         <v>1767</v>
       </c>
       <c r="B28">
@@ -15843,7 +15865,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="A29" t="s">
         <v>1768</v>
       </c>
       <c r="B29">
@@ -15851,7 +15873,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="A30" t="s">
         <v>1769</v>
       </c>
       <c r="B30">
@@ -15859,7 +15881,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="A31" t="s">
         <v>1770</v>
       </c>
       <c r="B31">
@@ -15867,7 +15889,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="A32" t="s">
         <v>1771</v>
       </c>
       <c r="B32">
@@ -15875,7 +15897,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="A33" t="s">
         <v>1772</v>
       </c>
       <c r="B33">
@@ -15883,7 +15905,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="A34" t="s">
         <v>1773</v>
       </c>
       <c r="B34">
@@ -15891,7 +15913,7 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="A35" t="s">
         <v>1774</v>
       </c>
       <c r="B35">
@@ -15899,7 +15921,7 @@
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
         <v>1775</v>
       </c>
       <c r="B36">
@@ -15907,7 +15929,7 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="A37" t="s">
         <v>1776</v>
       </c>
       <c r="B37">
@@ -15915,7 +15937,7 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="A38" t="s">
         <v>1777</v>
       </c>
       <c r="B38">
@@ -15923,7 +15945,7 @@
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="A39" t="s">
         <v>1778</v>
       </c>
       <c r="B39">
@@ -15931,7 +15953,7 @@
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="A40" t="s">
         <v>1779</v>
       </c>
       <c r="B40">
@@ -15939,7 +15961,7 @@
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="A41" t="s">
         <v>1780</v>
       </c>
       <c r="B41">

</xml_diff>